<commit_message>
Implemented weight and content filters
</commit_message>
<xml_diff>
--- a/Assets/Resources/SampleDataSet.xlsx
+++ b/Assets/Resources/SampleDataSet.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -10,7 +10,7 @@
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="0" documentId="8_{67475B7D-AFF4-4B99-B311-52D1DB83606F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="14235" xr2:uid="{E3715BC2-945D-4632-ADA5-FE9B4164C5E2}"/>
+    <workbookView activeTab="0" windowHeight="14235" windowWidth="21795" xWindow="-98" xr2:uid="{E3715BC2-945D-4632-ADA5-FE9B4164C5E2}" yWindow="-98"/>
   </bookViews>
   <sheets>
     <sheet name="Sayfa1" sheetId="1" r:id="rId1"/>
@@ -97,18 +97,37 @@
   <si>
     <t>HAFİF</t>
   </si>
+  <si>
+    <t>E1</t>
+  </si>
+  <si>
+    <t>E2</t>
+  </si>
+  <si>
+    <t>E3</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="8">
+    <numFmt numFmtId="5" formatCode="&quot;$&quot;#,##0_);(&quot;$&quot;#,##0)"/>
+    <numFmt numFmtId="6" formatCode="&quot;$&quot;#,##0_);[Red](&quot;$&quot;#,##0)"/>
+    <numFmt numFmtId="7" formatCode="&quot;$&quot;#,##0.00_);(&quot;$&quot;#,##0.00)"/>
+    <numFmt numFmtId="8" formatCode="&quot;$&quot;#,##0.00_);[Red](&quot;$&quot;#,##0.00)"/>
+    <numFmt numFmtId="41" formatCode="_(* #,##0_);_(* (#,##0);_(* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* (#,##0);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* (#,##0.00);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* (#,##0.00);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+  </numFmts>
+  <fonts count="1">
     <font>
+      <name val="Calibri"/>
+      <charset val="162"/>
+      <family val="2"/>
+      <color rgb="FF000000"/>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="162"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -122,15 +141,25 @@
   </fills>
   <borders count="1">
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
+      <left style="none">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="none">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="none">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="none">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal style="none">
+        <color rgb="FF000000"/>
+      </diagonal>
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -450,16 +479,15 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4C0C9011-2D51-445E-ADA4-5B11DDFBB09B}">
-  <dimension ref="A1:D13"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4C0C9011-2D51-445E-ADA4-5B11DDFBB09B}">
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:D1048576"/>
+    <sheetView workbookViewId="0" tabSelected="1">
+      <selection pane="topLeft" activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="14"/>
   <cols>
-    <col min="1" max="4" width="9.06640625" style="1"/>
+    <col min="1" max="4" width="9.06640625" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.45">
@@ -644,6 +672,48 @@
         <v>17</v>
       </c>
     </row>
+    <row r="14">
+      <c r="A14" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B14" s="1">
+        <v>40</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B15" s="1">
+        <v>15</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B16" s="1">
+        <v>60</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Code editing and scene improvement
</commit_message>
<xml_diff>
--- a/Assets/Resources/SampleDataSet.xlsx
+++ b/Assets/Resources/SampleDataSet.xlsx
@@ -112,11 +112,14 @@
   <si>
     <t>F2</t>
   </si>
+  <si>
+    <t>F3</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" count="8" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="8">
     <numFmt numFmtId="5" formatCode="&quot;$&quot;#,##0_);(&quot;$&quot;#,##0)"/>
     <numFmt numFmtId="6" formatCode="&quot;$&quot;#,##0_);[Red](&quot;$&quot;#,##0)"/>
@@ -488,7 +491,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4C0C9011-2D51-445E-ADA4-5B11DDFBB09B}">
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="1">
-      <selection pane="topLeft" activeCell="E18" sqref="E18"/>
+      <selection pane="topLeft" activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="14"/>
@@ -748,6 +751,17 @@
         <v>19</v>
       </c>
     </row>
+    <row r="19">
+      <c r="A19" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B19" s="1">
+        <v>20</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Revert "Code editing and scene improvement" git commit -m"Revert" q
This reverts commit 1f1cd6fe4adccb4c8ca14629d3db1b961c4b34cd.
</commit_message>
<xml_diff>
--- a/Assets/Resources/SampleDataSet.xlsx
+++ b/Assets/Resources/SampleDataSet.xlsx
@@ -112,14 +112,11 @@
   <si>
     <t>F2</t>
   </si>
-  <si>
-    <t>F3</t>
-  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" count="8" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="8">
     <numFmt numFmtId="5" formatCode="&quot;$&quot;#,##0_);(&quot;$&quot;#,##0)"/>
     <numFmt numFmtId="6" formatCode="&quot;$&quot;#,##0_);[Red](&quot;$&quot;#,##0)"/>
@@ -491,7 +488,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4C0C9011-2D51-445E-ADA4-5B11DDFBB09B}">
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="1">
-      <selection pane="topLeft" activeCell="C19" sqref="C19"/>
+      <selection pane="topLeft" activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="14"/>
@@ -751,17 +748,6 @@
         <v>19</v>
       </c>
     </row>
-    <row r="19">
-      <c r="A19" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="B19" s="1">
-        <v>20</v>
-      </c>
-      <c r="C19" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Code cleanup and scene improvement
</commit_message>
<xml_diff>
--- a/Assets/Resources/SampleDataSet.xlsx
+++ b/Assets/Resources/SampleDataSet.xlsx
@@ -114,6 +114,9 @@
   </si>
   <si>
     <t>F3</t>
+  </si>
+  <si>
+    <t>G1</t>
   </si>
 </sst>
 </file>
@@ -491,7 +494,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4C0C9011-2D51-445E-ADA4-5B11DDFBB09B}">
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="1">
-      <selection pane="topLeft" activeCell="C19" sqref="C19"/>
+      <selection pane="topLeft" activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="14"/>
@@ -761,6 +764,23 @@
       <c r="C19" s="1" t="s">
         <v>18</v>
       </c>
+      <c r="D19" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B20" s="1">
+        <v>10</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>17</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>